<commit_message>
OptimiZed the mail HTML
I have optimized the mail look included ever thing into HTML format
</commit_message>
<xml_diff>
--- a/Portfolio_Analyser.xlsx
+++ b/Portfolio_Analyser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,37 +536,37 @@
         <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>1.294994600688371</v>
+        <v>4.271044721348819</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8871226775507196</v>
+        <v>0.4106776180698152</v>
       </c>
       <c r="H2" t="n">
-        <v>-1.46686899342438</v>
+        <v>2.05071090941579</v>
       </c>
       <c r="I2" t="n">
-        <v>2.201648602269805</v>
+        <v>4.701028410921391</v>
       </c>
       <c r="J2" t="n">
-        <v>487</v>
+        <v>505.1000061035156</v>
       </c>
       <c r="K2" t="n">
-        <v>494.25</v>
+        <v>494.9500122070312</v>
       </c>
       <c r="L2" t="n">
-        <v>496.7000122070312</v>
+        <v>507.7999877929688</v>
       </c>
       <c r="M2" t="n">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N2" t="n">
         <v>2</v>
       </c>
       <c r="O2" t="n">
-        <v>490.3500061035156</v>
+        <v>487</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.683186715981894</v>
+        <v>3.716633696820457</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -595,37 +595,37 @@
         <v>12</v>
       </c>
       <c r="F3" t="n">
-        <v>1.893183044974469</v>
+        <v>1.433911123885336</v>
       </c>
       <c r="G3" t="n">
-        <v>0.303950038630642</v>
+        <v>0.3128535772193585</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.1215167005997362</v>
+        <v>0.3968930788753654</v>
       </c>
       <c r="I3" t="n">
-        <v>2.203831630697971</v>
+        <v>1.75224666748563</v>
       </c>
       <c r="J3" t="n">
-        <v>115.0699996948242</v>
+        <v>116.3600006103516</v>
       </c>
       <c r="K3" t="n">
-        <v>115.2099990844727</v>
+        <v>115.9000015258789</v>
       </c>
       <c r="L3" t="n">
-        <v>117.3300018310547</v>
+        <v>116.7200012207031</v>
       </c>
       <c r="M3" t="n">
-        <v>114.8000030517578</v>
+        <v>114.7099990844727</v>
       </c>
       <c r="N3" t="n">
         <v>2</v>
       </c>
       <c r="O3" t="n">
-        <v>115.1500015258789</v>
+        <v>115.0699996948242</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.06947618757669563</v>
+        <v>1.121057546665977</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -654,37 +654,37 @@
         <v>7</v>
       </c>
       <c r="F4" t="n">
-        <v>3.997943387469836</v>
+        <v>2.276751904357151</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2690974571240555</v>
+        <v>-0.01265325375448056</v>
       </c>
       <c r="H4" t="n">
-        <v>1.358971228966346</v>
+        <v>-0.5381711881062266</v>
       </c>
       <c r="I4" t="n">
-        <v>4.278554325485445</v>
+        <v>2.263812204699885</v>
       </c>
       <c r="J4" t="n">
-        <v>395.2999877929688</v>
+        <v>397.3500061035156</v>
       </c>
       <c r="K4" t="n">
-        <v>390</v>
+        <v>399.5</v>
       </c>
       <c r="L4" t="n">
-        <v>405.7999877929688</v>
+        <v>404.2999877929688</v>
       </c>
       <c r="M4" t="n">
-        <v>389.1499938964844</v>
+        <v>395.3500061035156</v>
       </c>
       <c r="N4" t="n">
         <v>2</v>
       </c>
       <c r="O4" t="n">
-        <v>390.2000122070312</v>
+        <v>395.2999877929688</v>
       </c>
       <c r="P4" t="n">
-        <v>1.307015742283362</v>
+        <v>0.518598121389403</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -713,37 +713,37 @@
         <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>1.462071457245358</v>
+        <v>2.266042520202404</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.0148397779614077</v>
+        <v>-0.3605079892651407</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7635796998585272</v>
+        <v>0.788324731979927</v>
       </c>
       <c r="I5" t="n">
-        <v>1.447016945182222</v>
+        <v>1.898689603226286</v>
       </c>
       <c r="J5" t="n">
-        <v>679.5999755859375</v>
+        <v>690.4000244140625</v>
       </c>
       <c r="K5" t="n">
-        <v>674.4500122070312</v>
+        <v>685</v>
       </c>
       <c r="L5" t="n">
-        <v>683.5499877929688</v>
+        <v>695</v>
       </c>
       <c r="M5" t="n">
-        <v>673.7999877929688</v>
+        <v>682.0499877929688</v>
       </c>
       <c r="N5" t="n">
         <v>2</v>
       </c>
       <c r="O5" t="n">
-        <v>673.7000122070312</v>
+        <v>679.5999755859375</v>
       </c>
       <c r="P5" t="n">
-        <v>0.8757552726736723</v>
+        <v>1.589177341981717</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -772,37 +772,37 @@
         <v>5</v>
       </c>
       <c r="F6" t="n">
-        <v>1.856264124810102</v>
+        <v>2.483816993976415</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7192345638006868</v>
+        <v>0.6103353718607099</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.8315799110814145</v>
+        <v>0.8705335094016572</v>
       </c>
       <c r="I6" t="n">
-        <v>2.59415676067272</v>
+        <v>3.113153040020527</v>
       </c>
       <c r="J6" t="n">
-        <v>188.4199981689453</v>
+        <v>191.1900024414062</v>
       </c>
       <c r="K6" t="n">
-        <v>190</v>
+        <v>189.5399932861328</v>
       </c>
       <c r="L6" t="n">
-        <v>192.6000061035156</v>
+        <v>193.1000061035156</v>
       </c>
       <c r="M6" t="n">
-        <v>187.7299957275391</v>
+        <v>187.2700042724609</v>
       </c>
       <c r="N6" t="n">
         <v>2</v>
       </c>
       <c r="O6" t="n">
-        <v>189.0899963378906</v>
+        <v>188.4199981689453</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.3543276650913211</v>
+        <v>1.470122226610593</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -831,37 +831,37 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1238163282027077</v>
+        <v>1.565591441326754</v>
       </c>
       <c r="G7" t="n">
-        <v>1.370568990128676</v>
+        <v>-0.02156473643322208</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.6640674928879049</v>
+        <v>1.054171462954937</v>
       </c>
       <c r="I7" t="n">
-        <v>1.515151515151515</v>
+        <v>1.543693811391769</v>
       </c>
       <c r="J7" t="n">
-        <v>2318.60009765625</v>
+        <v>2348.60009765625</v>
       </c>
       <c r="K7" t="n">
-        <v>2334.10009765625</v>
+        <v>2324.10009765625</v>
       </c>
       <c r="L7" t="n">
-        <v>2345</v>
+        <v>2354.89990234375</v>
       </c>
       <c r="M7" t="n">
-        <v>2310</v>
+        <v>2319.10009765625</v>
       </c>
       <c r="N7" t="n">
         <v>2</v>
       </c>
       <c r="O7" t="n">
-        <v>2342.10009765625</v>
+        <v>2318.60009765625</v>
       </c>
       <c r="P7" t="n">
-        <v>-1.003372999451072</v>
+        <v>1.293884185993325</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
@@ -890,37 +890,37 @@
         <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>1.544480510453737</v>
+        <v>1.387515882122624</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.2918132089635231</v>
+        <v>-0.5000686957151241</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4101873287217114</v>
+        <v>0.02096777275506639</v>
       </c>
       <c r="I8" t="n">
-        <v>1.249022488884723</v>
+        <v>0.8830314226893023</v>
       </c>
       <c r="J8" t="n">
-        <v>1419.800048828125</v>
+        <v>1431.300048828125</v>
       </c>
       <c r="K8" t="n">
-        <v>1414</v>
+        <v>1431</v>
       </c>
       <c r="L8" t="n">
-        <v>1426.699951171875</v>
+        <v>1439.5</v>
       </c>
       <c r="M8" t="n">
-        <v>1409.099975585938</v>
+        <v>1426.900024414062</v>
       </c>
       <c r="N8" t="n">
         <v>2</v>
       </c>
       <c r="O8" t="n">
-        <v>1405</v>
+        <v>1419.800048828125</v>
       </c>
       <c r="P8" t="n">
-        <v>1.053384258229537</v>
+        <v>0.8099732078113304</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -949,37 +949,37 @@
         <v>80</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9815469444041932</v>
+        <v>0.625243636022131</v>
       </c>
       <c r="G9" t="n">
-        <v>1.177853337841476</v>
+        <v>0.8206369307115923</v>
       </c>
       <c r="H9" t="n">
-        <v>1.386689321091944</v>
+        <v>-0.7410243027762784</v>
       </c>
       <c r="I9" t="n">
-        <v>2.18513800315224</v>
+        <v>1.457844174421252</v>
       </c>
       <c r="J9" t="n">
-        <v>25.59000015258789</v>
+        <v>25.45000076293945</v>
       </c>
       <c r="K9" t="n">
-        <v>25.23999977111816</v>
+        <v>25.63999938964844</v>
       </c>
       <c r="L9" t="n">
-        <v>25.71999931335449</v>
+        <v>25.75</v>
       </c>
       <c r="M9" t="n">
-        <v>25.17000007629395</v>
+        <v>25.3799991607666</v>
       </c>
       <c r="N9" t="n">
         <v>2</v>
       </c>
       <c r="O9" t="n">
-        <v>25.46999931335449</v>
+        <v>25.59000015258789</v>
       </c>
       <c r="P9" t="n">
-        <v>0.4711458283019243</v>
+        <v>-0.5470863181463463</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
@@ -1008,37 +1008,37 @@
         <v>8</v>
       </c>
       <c r="F10" t="n">
-        <v>1.893183044974469</v>
+        <v>1.433911123885336</v>
       </c>
       <c r="G10" t="n">
-        <v>0.303950038630642</v>
+        <v>0.3128535772193585</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.1215167005997362</v>
+        <v>0.3968930788753654</v>
       </c>
       <c r="I10" t="n">
-        <v>2.203831630697971</v>
+        <v>1.75224666748563</v>
       </c>
       <c r="J10" t="n">
-        <v>115.0699996948242</v>
+        <v>116.3600006103516</v>
       </c>
       <c r="K10" t="n">
-        <v>115.2099990844727</v>
+        <v>115.9000015258789</v>
       </c>
       <c r="L10" t="n">
-        <v>117.3300018310547</v>
+        <v>116.7200012207031</v>
       </c>
       <c r="M10" t="n">
-        <v>114.8000030517578</v>
+        <v>114.7099990844727</v>
       </c>
       <c r="N10" t="n">
         <v>3</v>
       </c>
       <c r="O10" t="n">
-        <v>115.1500015258789</v>
+        <v>115.0699996948242</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.06947618757669563</v>
+        <v>1.121057546665977</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1067,37 +1067,37 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4775653807555856</v>
+        <v>1.579837472285545</v>
       </c>
       <c r="G11" t="n">
-        <v>4.109590512174469</v>
+        <v>1.53414278958786</v>
       </c>
       <c r="H11" t="n">
-        <v>-3.962379383816614</v>
+        <v>0.2726355840230445</v>
       </c>
       <c r="I11" t="n">
-        <v>4.783748361730013</v>
+        <v>3.162497489072915</v>
       </c>
       <c r="J11" t="n">
-        <v>1531.800048828125</v>
+        <v>1544.699951171875</v>
       </c>
       <c r="K11" t="n">
-        <v>1595</v>
+        <v>1540.5</v>
       </c>
       <c r="L11" t="n">
-        <v>1599</v>
+        <v>1556</v>
       </c>
       <c r="M11" t="n">
-        <v>1526</v>
+        <v>1508.300048828125</v>
       </c>
       <c r="N11" t="n">
         <v>3</v>
       </c>
       <c r="O11" t="n">
-        <v>1591.400024414062</v>
+        <v>1531.800048828125</v>
       </c>
       <c r="P11" t="n">
-        <v>-3.745128482568775</v>
+        <v>0.8421400922149616</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -1126,37 +1126,37 @@
         <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7156959611269461</v>
+        <v>1.117373184419014</v>
       </c>
       <c r="G12" t="n">
-        <v>1.619745065141909</v>
+        <v>1.53990839568662</v>
       </c>
       <c r="H12" t="n">
-        <v>0.291927254418137</v>
+        <v>0.9895361002913892</v>
       </c>
       <c r="I12" t="n">
-        <v>2.37389202519881</v>
+        <v>2.698841263305531</v>
       </c>
       <c r="J12" t="n">
-        <v>1065</v>
+        <v>1061.400024414062</v>
       </c>
       <c r="K12" t="n">
-        <v>1061.900024414062</v>
+        <v>1051</v>
       </c>
       <c r="L12" t="n">
-        <v>1069.5</v>
+        <v>1076.900024414062</v>
       </c>
       <c r="M12" t="n">
-        <v>1044.699951171875</v>
+        <v>1048.599975585938</v>
       </c>
       <c r="N12" t="n">
         <v>3</v>
       </c>
       <c r="O12" t="n">
-        <v>1061.900024414062</v>
+        <v>1065</v>
       </c>
       <c r="P12" t="n">
-        <v>0.291927254418137</v>
+        <v>-0.3380258766138498</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
@@ -1185,37 +1185,37 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>3.34044065387349</v>
+        <v>3.352110956756162</v>
       </c>
       <c r="G13" t="n">
-        <v>1.066098081023454</v>
+        <v>0.267609072403169</v>
       </c>
       <c r="H13" t="n">
-        <v>1.428571428571429</v>
+        <v>2.276534607956529</v>
       </c>
       <c r="I13" t="n">
-        <v>4.454022988505748</v>
+        <v>3.629432720395879</v>
       </c>
       <c r="J13" t="n">
-        <v>355</v>
+        <v>366.1499938964844</v>
       </c>
       <c r="K13" t="n">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="L13" t="n">
-        <v>363.5</v>
+        <v>366.8999938964844</v>
       </c>
       <c r="M13" t="n">
-        <v>348</v>
+        <v>354.0499877929688</v>
       </c>
       <c r="N13" t="n">
         <v>3</v>
       </c>
       <c r="O13" t="n">
-        <v>351.75</v>
+        <v>355</v>
       </c>
       <c r="P13" t="n">
-        <v>0.9239516702203269</v>
+        <v>3.140843351122359</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -1244,37 +1244,37 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>5.045035910254782</v>
+        <v>2.716289488383365</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5945551323006577</v>
+        <v>0.8719000660907148</v>
       </c>
       <c r="H14" t="n">
-        <v>3.730761240388913</v>
+        <v>1.659856869532405</v>
       </c>
       <c r="I14" t="n">
-        <v>5.673322070095136</v>
+        <v>3.619750158498345</v>
       </c>
       <c r="J14" t="n">
-        <v>596.4000244140625</v>
+        <v>609.4000244140625</v>
       </c>
       <c r="K14" t="n">
-        <v>574.9500122070312</v>
+        <v>599.4500122070312</v>
       </c>
       <c r="L14" t="n">
-        <v>600.7000122070312</v>
+        <v>612.5999755859375</v>
       </c>
       <c r="M14" t="n">
-        <v>568.4500122070312</v>
+        <v>591.2000122070312</v>
       </c>
       <c r="N14" t="n">
         <v>3</v>
       </c>
       <c r="O14" t="n">
-        <v>571.8499755859375</v>
+        <v>596.4000244140625</v>
       </c>
       <c r="P14" t="n">
-        <v>4.293092572570307</v>
+        <v>2.179745048262187</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
@@ -1303,37 +1303,37 @@
         <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1238163282027077</v>
+        <v>1.565591441326754</v>
       </c>
       <c r="G15" t="n">
-        <v>1.370568990128676</v>
+        <v>-0.02156473643322208</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.6640674928879049</v>
+        <v>1.054171462954937</v>
       </c>
       <c r="I15" t="n">
-        <v>1.515151515151515</v>
+        <v>1.543693811391769</v>
       </c>
       <c r="J15" t="n">
-        <v>2318.60009765625</v>
+        <v>2348.60009765625</v>
       </c>
       <c r="K15" t="n">
-        <v>2334.10009765625</v>
+        <v>2324.10009765625</v>
       </c>
       <c r="L15" t="n">
-        <v>2345</v>
+        <v>2354.89990234375</v>
       </c>
       <c r="M15" t="n">
-        <v>2310</v>
+        <v>2319.10009765625</v>
       </c>
       <c r="N15" t="n">
         <v>3</v>
       </c>
       <c r="O15" t="n">
-        <v>2342.10009765625</v>
+        <v>2318.60009765625</v>
       </c>
       <c r="P15" t="n">
-        <v>-1.003372999451072</v>
+        <v>1.293884185993325</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
@@ -1362,37 +1362,37 @@
         <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>2.696871654277082</v>
+        <v>2.249053379274764</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.09246040862703582</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>1.923076923076923</v>
+        <v>0.9489339647684922</v>
       </c>
       <c r="I16" t="n">
-        <v>2.602005420805471</v>
+        <v>2.249053379274764</v>
       </c>
       <c r="J16" t="n">
+        <v>67.01999664306641</v>
+      </c>
+      <c r="K16" t="n">
+        <v>66.38999938964844</v>
+      </c>
+      <c r="L16" t="n">
+        <v>67.73999786376953</v>
+      </c>
+      <c r="M16" t="n">
         <v>66.25</v>
-      </c>
-      <c r="K16" t="n">
-        <v>65</v>
-      </c>
-      <c r="L16" t="n">
-        <v>66.63999938964844</v>
-      </c>
-      <c r="M16" t="n">
-        <v>64.94999694824219</v>
       </c>
       <c r="N16" t="n">
         <v>3</v>
       </c>
       <c r="O16" t="n">
-        <v>64.88999938964844</v>
+        <v>66.25</v>
       </c>
       <c r="P16" t="n">
-        <v>2.095855483346662</v>
+        <v>1.162259083873821</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
@@ -1421,37 +1421,37 @@
         <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>2.503601386119635</v>
+        <v>5.706024954921772</v>
       </c>
       <c r="G17" t="n">
-        <v>1.258361032098139</v>
+        <v>0.3286878885414234</v>
       </c>
       <c r="H17" t="n">
-        <v>-1.220782391436688</v>
+        <v>3.411459922790527</v>
       </c>
       <c r="I17" t="n">
-        <v>3.809904775269815</v>
+        <v>6.054613625147033</v>
       </c>
       <c r="J17" t="n">
-        <v>380.2999877929688</v>
+        <v>397.1000061035156</v>
       </c>
       <c r="K17" t="n">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L17" t="n">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="M17" t="n">
-        <v>376.6499938964844</v>
+        <v>379.0499877929688</v>
       </c>
       <c r="N17" t="n">
         <v>3</v>
       </c>
       <c r="O17" t="n">
-        <v>381.4500122070312</v>
+        <v>380.2999877929688</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.3014875808781798</v>
+        <v>4.417570036760723</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -1480,37 +1480,37 @@
         <v>18</v>
       </c>
       <c r="F18" t="n">
-        <v>1.816032345861871</v>
+        <v>2.751384356796515</v>
       </c>
       <c r="G18" t="n">
-        <v>0.6119253340401491</v>
+        <v>-0.03958918761371132</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.4532010684459667</v>
+        <v>1.469147916177687</v>
       </c>
       <c r="I18" t="n">
-        <v>2.442906443315567</v>
+        <v>2.710722016358062</v>
       </c>
       <c r="J18" t="n">
-        <v>50.52000045776367</v>
+        <v>51.79999923706055</v>
       </c>
       <c r="K18" t="n">
-        <v>50.75</v>
+        <v>51.04999923706055</v>
       </c>
       <c r="L18" t="n">
-        <v>51.58000183105469</v>
+        <v>51.90999984741211</v>
       </c>
       <c r="M18" t="n">
-        <v>50.34999847412109</v>
+        <v>50.54000091552734</v>
       </c>
       <c r="N18" t="n">
         <v>3</v>
       </c>
       <c r="O18" t="n">
-        <v>50.65999984741211</v>
+        <v>50.52000045776367</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.2763509476314954</v>
+        <v>2.533647600353834</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
@@ -1539,37 +1539,37 @@
         <v>2</v>
       </c>
       <c r="F19" t="n">
-        <v>1.544480510453737</v>
+        <v>1.387515882122624</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.2918132089635231</v>
+        <v>-0.5000686957151241</v>
       </c>
       <c r="H19" t="n">
-        <v>0.4101873287217114</v>
+        <v>0.02096777275506639</v>
       </c>
       <c r="I19" t="n">
-        <v>1.249022488884723</v>
+        <v>0.8830314226893023</v>
       </c>
       <c r="J19" t="n">
-        <v>1419.800048828125</v>
+        <v>1431.300048828125</v>
       </c>
       <c r="K19" t="n">
-        <v>1414</v>
+        <v>1431</v>
       </c>
       <c r="L19" t="n">
-        <v>1426.699951171875</v>
+        <v>1439.5</v>
       </c>
       <c r="M19" t="n">
-        <v>1409.099975585938</v>
+        <v>1426.900024414062</v>
       </c>
       <c r="N19" t="n">
         <v>3</v>
       </c>
       <c r="O19" t="n">
-        <v>1405</v>
+        <v>1419.800048828125</v>
       </c>
       <c r="P19" t="n">
-        <v>1.053384258229537</v>
+        <v>0.8099732078113304</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
@@ -1598,37 +1598,37 @@
         <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>2.7965881019957</v>
+        <v>2.078173360513444</v>
       </c>
       <c r="G20" t="n">
-        <v>1.231203532803545</v>
+        <v>-0.03537399617936553</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.5452903551701328</v>
+        <v>0.692983259234512</v>
       </c>
       <c r="I20" t="n">
-        <v>4.078000116298849</v>
+        <v>2.042077000094086</v>
       </c>
       <c r="J20" t="n">
-        <v>113.0800018310547</v>
+        <v>114.7900009155273</v>
       </c>
       <c r="K20" t="n">
-        <v>113.6999969482422</v>
+        <v>114</v>
       </c>
       <c r="L20" t="n">
-        <v>116.8899993896484</v>
+        <v>115.4300003051758</v>
       </c>
       <c r="M20" t="n">
-        <v>112.3099975585938</v>
+        <v>113.120002746582</v>
       </c>
       <c r="N20" t="n">
         <v>3</v>
       </c>
       <c r="O20" t="n">
-        <v>113.7099990844727</v>
+        <v>113.0800018310547</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.5540385704778326</v>
+        <v>1.512202915443397</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
@@ -1657,37 +1657,37 @@
         <v>35</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9815469444041932</v>
+        <v>0.625243636022131</v>
       </c>
       <c r="G21" t="n">
-        <v>1.177853337841476</v>
+        <v>0.8206369307115923</v>
       </c>
       <c r="H21" t="n">
-        <v>1.386689321091944</v>
+        <v>-0.7410243027762784</v>
       </c>
       <c r="I21" t="n">
-        <v>2.18513800315224</v>
+        <v>1.457844174421252</v>
       </c>
       <c r="J21" t="n">
-        <v>25.59000015258789</v>
+        <v>25.45000076293945</v>
       </c>
       <c r="K21" t="n">
-        <v>25.23999977111816</v>
+        <v>25.63999938964844</v>
       </c>
       <c r="L21" t="n">
-        <v>25.71999931335449</v>
+        <v>25.75</v>
       </c>
       <c r="M21" t="n">
-        <v>25.17000007629395</v>
+        <v>25.3799991607666</v>
       </c>
       <c r="N21" t="n">
         <v>3</v>
       </c>
       <c r="O21" t="n">
-        <v>25.46999931335449</v>
+        <v>25.59000015258789</v>
       </c>
       <c r="P21" t="n">
-        <v>0.4711458283019243</v>
+        <v>-0.5470863181463463</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
@@ -1716,37 +1716,37 @@
         <v>2</v>
       </c>
       <c r="F22" t="n">
-        <v>2.654245337359333</v>
+        <v>2.703751269175863</v>
       </c>
       <c r="G22" t="n">
-        <v>1.350409345290066</v>
+        <v>-1.039901441054104</v>
       </c>
       <c r="H22" t="n">
-        <v>1.263646737275741</v>
+        <v>-0.2111809922744657</v>
       </c>
       <c r="I22" t="n">
-        <v>4.059474201637957</v>
+        <v>1.646725505856155</v>
       </c>
       <c r="J22" t="n">
-        <v>649.0999755859375</v>
+        <v>661.5499877929688</v>
       </c>
       <c r="K22" t="n">
-        <v>641</v>
+        <v>662.9500122070312</v>
       </c>
       <c r="L22" t="n">
-        <v>661.3499755859375</v>
+        <v>666.6500244140625</v>
       </c>
       <c r="M22" t="n">
-        <v>635.5499877929688</v>
+        <v>655.8499755859375</v>
       </c>
       <c r="N22" t="n">
         <v>3</v>
       </c>
       <c r="O22" t="n">
-        <v>644.25</v>
+        <v>649.0999755859375</v>
       </c>
       <c r="P22" t="n">
-        <v>0.752809559322856</v>
+        <v>1.918042316330812</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -1775,37 +1775,37 @@
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>1.094479814765005</v>
+        <v>2.142232585252113</v>
       </c>
       <c r="G23" t="n">
-        <v>0.9757637214674734</v>
+        <v>-0.448845885856893</v>
       </c>
       <c r="H23" t="n">
-        <v>-1.180875576036866</v>
+        <v>0.1246390964673913</v>
       </c>
       <c r="I23" t="n">
-        <v>2.090643274853801</v>
+        <v>1.685819965835613</v>
       </c>
       <c r="J23" t="n">
-        <v>3431</v>
+        <v>3454.300048828125</v>
       </c>
       <c r="K23" t="n">
-        <v>3472</v>
+        <v>3450</v>
       </c>
       <c r="L23" t="n">
-        <v>3491.5</v>
+        <v>3504.5</v>
       </c>
       <c r="M23" t="n">
-        <v>3420</v>
+        <v>3446.39990234375</v>
       </c>
       <c r="N23" t="n">
         <v>3</v>
       </c>
       <c r="O23" t="n">
-        <v>3453.699951171875</v>
+        <v>3431</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.657264715893246</v>
+        <v>0.6791037256812882</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
@@ -1834,37 +1834,37 @@
         <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>3.123393146729601</v>
+        <v>1.069796234332024</v>
       </c>
       <c r="G24" t="n">
-        <v>1.484899668875304</v>
+        <v>1.324494817365288</v>
       </c>
       <c r="H24" t="n">
-        <v>1.18556467401494</v>
+        <v>-0.3042569372796623</v>
       </c>
       <c r="I24" t="n">
-        <v>4.677752750711018</v>
+        <v>2.426428977754723</v>
       </c>
       <c r="J24" t="n">
-        <v>19.6299991607666</v>
+        <v>19.65999984741211</v>
       </c>
       <c r="K24" t="n">
-        <v>19.39999961853027</v>
+        <v>19.71999931335449</v>
       </c>
       <c r="L24" t="n">
-        <v>20.13999938964844</v>
+        <v>19.84000015258789</v>
       </c>
       <c r="M24" t="n">
-        <v>19.23999977111816</v>
+        <v>19.3700008392334</v>
       </c>
       <c r="N24" t="n">
         <v>4</v>
       </c>
       <c r="O24" t="n">
-        <v>19.53000068664551</v>
+        <v>19.6299991607666</v>
       </c>
       <c r="P24" t="n">
-        <v>0.5120249390952254</v>
+        <v>0.1528308096185176</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
@@ -1893,37 +1893,37 @@
         <v>3</v>
       </c>
       <c r="F25" t="n">
-        <v>4.715612721198091</v>
+        <v>2.527653667635449</v>
       </c>
       <c r="G25" t="n">
-        <v>2.698950218867168</v>
+        <v>0.3090043925245983</v>
       </c>
       <c r="H25" t="n">
-        <v>-4.027288433639202</v>
+        <v>1.475217252444011</v>
       </c>
       <c r="I25" t="n">
-        <v>7.620229130871083</v>
+        <v>2.845450627586408</v>
       </c>
       <c r="J25" t="n">
-        <v>161.8099975585938</v>
+        <v>164.3999938964844</v>
       </c>
       <c r="K25" t="n">
-        <v>168.6000061035156</v>
+        <v>162.0099945068359</v>
       </c>
       <c r="L25" t="n">
-        <v>173.4299926757812</v>
+        <v>165.8999938964844</v>
       </c>
       <c r="M25" t="n">
-        <v>161.1499938964844</v>
+        <v>161.3099975585938</v>
       </c>
       <c r="N25" t="n">
         <v>4</v>
       </c>
       <c r="O25" t="n">
-        <v>165.6199951171875</v>
+        <v>161.8099975585938</v>
       </c>
       <c r="P25" t="n">
-        <v>-2.300445399661989</v>
+        <v>1.600640490061654</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
@@ -1952,37 +1952,37 @@
         <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>0.8642434783373176</v>
+        <v>1.292458094258014</v>
       </c>
       <c r="G26" t="n">
-        <v>1.444398614553441</v>
+        <v>0.03231222272224098</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.765532529903557</v>
+        <v>0.2131933894950053</v>
       </c>
       <c r="I26" t="n">
-        <v>2.342476795267843</v>
+        <v>1.325198518076928</v>
       </c>
       <c r="J26" t="n">
-        <v>247.5899963378906</v>
+        <v>249.1300048828125</v>
       </c>
       <c r="K26" t="n">
-        <v>249.5</v>
+        <v>248.6000061035156</v>
       </c>
       <c r="L26" t="n">
-        <v>252.0899963378906</v>
+        <v>250.7899932861328</v>
       </c>
       <c r="M26" t="n">
-        <v>246.3200073242188</v>
+        <v>247.5099945068359</v>
       </c>
       <c r="N26" t="n">
         <v>4</v>
       </c>
       <c r="O26" t="n">
-        <v>249.9299926757812</v>
+        <v>247.5899963378906</v>
       </c>
       <c r="P26" t="n">
-        <v>-0.9362607155861272</v>
+        <v>0.62199950228207</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
@@ -2011,37 +2011,37 @@
         <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>1.935284544401637</v>
+        <v>2.072678745789038</v>
       </c>
       <c r="G27" t="n">
-        <v>1.137366369558406</v>
+        <v>-0.07561187010666628</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.8860847025592172</v>
+        <v>1.653333875868055</v>
       </c>
       <c r="I27" t="n">
-        <v>3.108000263725443</v>
+        <v>1.995557996961806</v>
       </c>
       <c r="J27" t="n">
-        <v>224.8300018310547</v>
+        <v>228.7200012207031</v>
       </c>
       <c r="K27" t="n">
-        <v>226.8399963378906</v>
+        <v>225</v>
       </c>
       <c r="L27" t="n">
-        <v>231.2299957275391</v>
+        <v>229.4900054931641</v>
       </c>
       <c r="M27" t="n">
-        <v>224.2599945068359</v>
+        <v>225</v>
       </c>
       <c r="N27" t="n">
         <v>4</v>
       </c>
       <c r="O27" t="n">
-        <v>226.8399963378906</v>
+        <v>224.8300018310547</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.8860847025592172</v>
+        <v>1.730195862637373</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
@@ -2070,37 +2070,37 @@
         <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>1.848749840010016</v>
+        <v>4.015624523162842</v>
       </c>
       <c r="G28" t="n">
-        <v>3.254388621442365</v>
+        <v>0.7343769073486328</v>
       </c>
       <c r="H28" t="n">
-        <v>-1.234572552595136</v>
+        <v>1.884462868334252</v>
       </c>
       <c r="I28" t="n">
-        <v>5.274800984495533</v>
+        <v>4.785142411364279</v>
       </c>
       <c r="J28" t="n">
-        <v>64</v>
+        <v>65.95999908447266</v>
       </c>
       <c r="K28" t="n">
-        <v>64.80000305175781</v>
+        <v>64.73999786376953</v>
       </c>
       <c r="L28" t="n">
-        <v>66.66000366210938</v>
+        <v>66.56999969482422</v>
       </c>
       <c r="M28" t="n">
-        <v>63.31999969482422</v>
+        <v>63.52999877929688</v>
       </c>
       <c r="N28" t="n">
         <v>4</v>
       </c>
       <c r="O28" t="n">
-        <v>65.44999694824219</v>
+        <v>64</v>
       </c>
       <c r="P28" t="n">
-        <v>-2.215427067764181</v>
+        <v>3.062498569488525</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
@@ -2129,37 +2129,37 @@
         <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>1.559778676307445</v>
+        <v>1.11731239472683</v>
       </c>
       <c r="G29" t="n">
-        <v>1.026167297399837</v>
+        <v>0.01034775072576329</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.8615347055288461</v>
+        <v>0.1649522289787371</v>
       </c>
       <c r="I29" t="n">
-        <v>2.61275723400307</v>
+        <v>1.127776844989256</v>
       </c>
       <c r="J29" t="n">
-        <v>96.66000366210938</v>
+        <v>97.16000366210938</v>
       </c>
       <c r="K29" t="n">
-        <v>97.5</v>
+        <v>97</v>
       </c>
       <c r="L29" t="n">
-        <v>98.97000122070312</v>
+        <v>97.73999786376953</v>
       </c>
       <c r="M29" t="n">
-        <v>96.44999694824219</v>
+        <v>96.65000152587891</v>
       </c>
       <c r="N29" t="n">
         <v>4</v>
       </c>
       <c r="O29" t="n">
-        <v>97.44999694824219</v>
+        <v>96.66000366210938</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.8106652753949238</v>
+        <v>0.5172770339920849</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
@@ -2188,37 +2188,37 @@
         <v>2</v>
       </c>
       <c r="F30" t="n">
-        <v>0.4775653807555856</v>
+        <v>1.579837472285545</v>
       </c>
       <c r="G30" t="n">
-        <v>4.109590512174469</v>
+        <v>1.53414278958786</v>
       </c>
       <c r="H30" t="n">
-        <v>-3.962379383816614</v>
+        <v>0.2726355840230445</v>
       </c>
       <c r="I30" t="n">
-        <v>4.783748361730013</v>
+        <v>3.162497489072915</v>
       </c>
       <c r="J30" t="n">
-        <v>1531.800048828125</v>
+        <v>1544.699951171875</v>
       </c>
       <c r="K30" t="n">
-        <v>1595</v>
+        <v>1540.5</v>
       </c>
       <c r="L30" t="n">
-        <v>1599</v>
+        <v>1556</v>
       </c>
       <c r="M30" t="n">
-        <v>1526</v>
+        <v>1508.300048828125</v>
       </c>
       <c r="N30" t="n">
         <v>4</v>
       </c>
       <c r="O30" t="n">
-        <v>1591.400024414062</v>
+        <v>1531.800048828125</v>
       </c>
       <c r="P30" t="n">
-        <v>-3.745128482568775</v>
+        <v>0.8421400922149616</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
@@ -2247,37 +2247,37 @@
         <v>5</v>
       </c>
       <c r="F31" t="n">
-        <v>2.635552780031655</v>
+        <v>0.2009332131047441</v>
       </c>
       <c r="G31" t="n">
-        <v>1.004536926746771</v>
+        <v>2.167930917186212</v>
       </c>
       <c r="H31" t="n">
-        <v>1.677416729670699</v>
+        <v>-0.7454787713116245</v>
       </c>
       <c r="I31" t="n">
-        <v>3.677026798778531</v>
+        <v>2.42135748788645</v>
       </c>
       <c r="J31" t="n">
-        <v>94.55999755859375</v>
+        <v>93.19999694824219</v>
       </c>
       <c r="K31" t="n">
-        <v>93</v>
+        <v>93.90000152587891</v>
       </c>
       <c r="L31" t="n">
-        <v>95.01999664306641</v>
+        <v>94.75</v>
       </c>
       <c r="M31" t="n">
-        <v>91.65000152587891</v>
+        <v>92.51000213623047</v>
       </c>
       <c r="N31" t="n">
         <v>4</v>
       </c>
       <c r="O31" t="n">
-        <v>92.58000183105469</v>
+        <v>94.55999755859375</v>
       </c>
       <c r="P31" t="n">
-        <v>2.138686204772681</v>
+        <v>-1.43824095332579</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
@@ -2306,37 +2306,37 @@
         <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>3.020407229053731</v>
+        <v>1.673769015247799</v>
       </c>
       <c r="G32" t="n">
-        <v>0.8775516432158801</v>
+        <v>1.907085461445245</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.5247191231816192</v>
+        <v>-2.197802451374629</v>
       </c>
       <c r="I32" t="n">
-        <v>3.932468312565473</v>
+        <v>3.650472099374327</v>
       </c>
       <c r="J32" t="n">
-        <v>98.58000183105469</v>
+        <v>97.01000213623047</v>
       </c>
       <c r="K32" t="n">
-        <v>99.09999847412109</v>
+        <v>99.19000244140625</v>
       </c>
       <c r="L32" t="n">
-        <v>100.9599990844727</v>
+        <v>100.2300033569336</v>
       </c>
       <c r="M32" t="n">
-        <v>97.13999938964844</v>
+        <v>96.69999694824219</v>
       </c>
       <c r="N32" t="n">
         <v>4</v>
       </c>
       <c r="O32" t="n">
-        <v>98</v>
+        <v>98.58000183105469</v>
       </c>
       <c r="P32" t="n">
-        <v>0.5918386031170281</v>
+        <v>-1.592614795762397</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
@@ -2365,37 +2365,37 @@
         <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>3.34044065387349</v>
+        <v>3.352110956756162</v>
       </c>
       <c r="G33" t="n">
-        <v>1.066098081023454</v>
+        <v>0.267609072403169</v>
       </c>
       <c r="H33" t="n">
-        <v>1.428571428571429</v>
+        <v>2.276534607956529</v>
       </c>
       <c r="I33" t="n">
-        <v>4.454022988505748</v>
+        <v>3.629432720395879</v>
       </c>
       <c r="J33" t="n">
-        <v>355</v>
+        <v>366.1499938964844</v>
       </c>
       <c r="K33" t="n">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="L33" t="n">
-        <v>363.5</v>
+        <v>366.8999938964844</v>
       </c>
       <c r="M33" t="n">
-        <v>348</v>
+        <v>354.0499877929688</v>
       </c>
       <c r="N33" t="n">
         <v>4</v>
       </c>
       <c r="O33" t="n">
-        <v>351.75</v>
+        <v>355</v>
       </c>
       <c r="P33" t="n">
-        <v>0.9239516702203269</v>
+        <v>3.140843351122359</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
@@ -2424,37 +2424,37 @@
         <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>1.15841301517748</v>
+        <v>2.846715328467153</v>
       </c>
       <c r="G34" t="n">
-        <v>1.607294523362784</v>
+        <v>0.364963503649635</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.8108855754282669</v>
+        <v>3.03296882154304</v>
       </c>
       <c r="I34" t="n">
-        <v>2.810886767614055</v>
+        <v>3.223443223443224</v>
       </c>
       <c r="J34" t="n">
-        <v>1370</v>
+        <v>1406.400024414062</v>
       </c>
       <c r="K34" t="n">
-        <v>1381.199951171875</v>
+        <v>1365</v>
       </c>
       <c r="L34" t="n">
-        <v>1397.199951171875</v>
+        <v>1409</v>
       </c>
       <c r="M34" t="n">
-        <v>1359</v>
+        <v>1365</v>
       </c>
       <c r="N34" t="n">
         <v>4</v>
       </c>
       <c r="O34" t="n">
-        <v>1381.199951171875</v>
+        <v>1370</v>
       </c>
       <c r="P34" t="n">
-        <v>-0.8108855754282669</v>
+        <v>2.656936088617701</v>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
@@ -2483,37 +2483,37 @@
         <v>4</v>
       </c>
       <c r="F35" t="n">
-        <v>0.8779233461850648</v>
+        <v>1.566157198791555</v>
       </c>
       <c r="G35" t="n">
-        <v>0.2597402597402597</v>
+        <v>-0.5411324357120604</v>
       </c>
       <c r="H35" t="n">
-        <v>-0.4093701012630716</v>
+        <v>-0.113458028461836</v>
       </c>
       <c r="I35" t="n">
-        <v>1.140626271565755</v>
+        <v>1.019507875281707</v>
       </c>
       <c r="J35" t="n">
-        <v>1921.900024414062</v>
+        <v>1936.800048828125</v>
       </c>
       <c r="K35" t="n">
-        <v>1929.800048828125</v>
+        <v>1939</v>
       </c>
       <c r="L35" t="n">
-        <v>1941.900024414062</v>
+        <v>1952</v>
       </c>
       <c r="M35" t="n">
-        <v>1920</v>
+        <v>1932.300048828125</v>
       </c>
       <c r="N35" t="n">
         <v>4</v>
       </c>
       <c r="O35" t="n">
-        <v>1925</v>
+        <v>1921.900024414062</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.161037692775974</v>
+        <v>0.7752757284346844</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
@@ -2542,37 +2542,37 @@
         <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>1.373509151081815</v>
+        <v>1.167755648366135</v>
       </c>
       <c r="G36" t="n">
-        <v>0.1681867143701822</v>
+        <v>0.2866915359716489</v>
       </c>
       <c r="H36" t="n">
-        <v>0.2242589611832838</v>
+        <v>-0.7361094156901042</v>
       </c>
       <c r="I36" t="n">
-        <v>1.544293161380366</v>
+        <v>1.458628950078892</v>
       </c>
       <c r="J36" t="n">
-        <v>1430.099975585938</v>
+        <v>1429.400024414062</v>
       </c>
       <c r="K36" t="n">
-        <v>1426.900024414062</v>
+        <v>1440</v>
       </c>
       <c r="L36" t="n">
-        <v>1446.599975585938</v>
+        <v>1446.800048828125</v>
       </c>
       <c r="M36" t="n">
-        <v>1424.599975585938</v>
+        <v>1426</v>
       </c>
       <c r="N36" t="n">
         <v>4</v>
       </c>
       <c r="O36" t="n">
-        <v>1427</v>
+        <v>1430.099975585938</v>
       </c>
       <c r="P36" t="n">
-        <v>0.2172372519928171</v>
+        <v>-0.04894421256025947</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
@@ -2601,37 +2601,37 @@
         <v>5</v>
       </c>
       <c r="F37" t="n">
-        <v>1.014653062777023</v>
+        <v>3.185995041710429</v>
       </c>
       <c r="G37" t="n">
-        <v>0.7265461828275455</v>
+        <v>-0.01258595438235246</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.5510267005882517</v>
+        <v>1.011864494333662</v>
       </c>
       <c r="I37" t="n">
-        <v>1.753942447505915</v>
+        <v>3.173009733770437</v>
       </c>
       <c r="J37" t="n">
-        <v>79.41000366210938</v>
+        <v>80.86000061035156</v>
       </c>
       <c r="K37" t="n">
-        <v>79.84999847412109</v>
+        <v>80.05000305175781</v>
       </c>
       <c r="L37" t="n">
-        <v>80.63999938964844</v>
+        <v>81.94000244140625</v>
       </c>
       <c r="M37" t="n">
-        <v>79.25</v>
+        <v>79.41999816894531</v>
       </c>
       <c r="N37" t="n">
         <v>4</v>
       </c>
       <c r="O37" t="n">
-        <v>79.83000183105469</v>
+        <v>79.41000366210938</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.5261156949916652</v>
+        <v>1.825962575712682</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -2660,37 +2660,37 @@
         <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>1.685391678200277</v>
+        <v>1.843966440945715</v>
       </c>
       <c r="G38" t="n">
-        <v>1.264040410074605</v>
+        <v>0.5673753300829047</v>
       </c>
       <c r="H38" t="n">
-        <v>-0.9831417970412254</v>
+        <v>0.9887030002217159</v>
       </c>
       <c r="I38" t="n">
-        <v>2.987191394629267</v>
+        <v>2.425101196949657</v>
       </c>
       <c r="J38" t="n">
-        <v>7.050000190734863</v>
+        <v>7.150000095367432</v>
       </c>
       <c r="K38" t="n">
-        <v>7.119999885559082</v>
+        <v>7.079999923706055</v>
       </c>
       <c r="L38" t="n">
-        <v>7.239999771118164</v>
+        <v>7.179999828338623</v>
       </c>
       <c r="M38" t="n">
-        <v>7.03000020980835</v>
+        <v>7.010000228881836</v>
       </c>
       <c r="N38" t="n">
         <v>4</v>
       </c>
       <c r="O38" t="n">
-        <v>7.119999885559082</v>
+        <v>7.050000190734863</v>
       </c>
       <c r="P38" t="n">
-        <v>-0.9831417970412254</v>
+        <v>1.418438325207262</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
@@ -2719,37 +2719,37 @@
         <v>11</v>
       </c>
       <c r="F39" t="n">
-        <v>2.696871654277082</v>
+        <v>2.249053379274764</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.09246040862703582</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>1.923076923076923</v>
+        <v>0.9489339647684922</v>
       </c>
       <c r="I39" t="n">
-        <v>2.602005420805471</v>
+        <v>2.249053379274764</v>
       </c>
       <c r="J39" t="n">
+        <v>67.01999664306641</v>
+      </c>
+      <c r="K39" t="n">
+        <v>66.38999938964844</v>
+      </c>
+      <c r="L39" t="n">
+        <v>67.73999786376953</v>
+      </c>
+      <c r="M39" t="n">
         <v>66.25</v>
-      </c>
-      <c r="K39" t="n">
-        <v>65</v>
-      </c>
-      <c r="L39" t="n">
-        <v>66.63999938964844</v>
-      </c>
-      <c r="M39" t="n">
-        <v>64.94999694824219</v>
       </c>
       <c r="N39" t="n">
         <v>4</v>
       </c>
       <c r="O39" t="n">
-        <v>64.88999938964844</v>
+        <v>66.25</v>
       </c>
       <c r="P39" t="n">
-        <v>2.095855483346662</v>
+        <v>1.162259083873821</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
@@ -2778,37 +2778,37 @@
         <v>5</v>
       </c>
       <c r="F40" t="n">
-        <v>1.912266494842634</v>
+        <v>3.128119850969529</v>
       </c>
       <c r="G40" t="n">
-        <v>0.6409252332987408</v>
+        <v>0.1469578444816008</v>
       </c>
       <c r="H40" t="n">
-        <v>0.09455879695815028</v>
+        <v>1.90078297109579</v>
       </c>
       <c r="I40" t="n">
-        <v>2.569661336054469</v>
+        <v>3.279897762504107</v>
       </c>
       <c r="J40" t="n">
-        <v>190.5299987792969</v>
+        <v>195.1399993896484</v>
       </c>
       <c r="K40" t="n">
-        <v>190.3500061035156</v>
+        <v>191.5</v>
       </c>
       <c r="L40" t="n">
-        <v>193.9900054931641</v>
+        <v>196.4900054931641</v>
       </c>
       <c r="M40" t="n">
-        <v>189.1300048828125</v>
+        <v>190.25</v>
       </c>
       <c r="N40" t="n">
         <v>4</v>
       </c>
       <c r="O40" t="n">
-        <v>190.3500061035156</v>
+        <v>190.5299987792969</v>
       </c>
       <c r="P40" t="n">
-        <v>0.09455879695815028</v>
+        <v>2.419566808317478</v>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
@@ -2837,37 +2837,37 @@
         <v>2</v>
       </c>
       <c r="F41" t="n">
-        <v>1.338659551536365</v>
+        <v>2.09545983701979</v>
       </c>
       <c r="G41" t="n">
-        <v>0.39924418463809</v>
+        <v>0.03492290954234575</v>
       </c>
       <c r="H41" t="n">
-        <v>1.273283145194374</v>
+        <v>1.557237003377397</v>
       </c>
       <c r="I41" t="n">
-        <v>1.744870028291903</v>
+        <v>2.131126998115921</v>
       </c>
       <c r="J41" t="n">
-        <v>429.5</v>
+        <v>436.9500122070312</v>
       </c>
       <c r="K41" t="n">
-        <v>424.1000061035156</v>
+        <v>430.25</v>
       </c>
       <c r="L41" t="n">
-        <v>431.5</v>
+        <v>438.5</v>
       </c>
       <c r="M41" t="n">
-        <v>424.1000061035156</v>
+        <v>429.3500061035156</v>
       </c>
       <c r="N41" t="n">
         <v>4</v>
       </c>
       <c r="O41" t="n">
-        <v>425.7999877929688</v>
+        <v>429.5</v>
       </c>
       <c r="P41" t="n">
-        <v>0.8689554516451182</v>
+        <v>1.734577929460128</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
@@ -2896,37 +2896,37 @@
         <v>6</v>
       </c>
       <c r="F42" t="n">
-        <v>0.6058107691572595</v>
+        <v>2.026856016759221</v>
       </c>
       <c r="G42" t="n">
-        <v>4.862875454117608</v>
+        <v>1.650560420883153</v>
       </c>
       <c r="H42" t="n">
-        <v>-3.443433708908292</v>
+        <v>0.3399350149598898</v>
       </c>
       <c r="I42" t="n">
-        <v>5.748214747269821</v>
+        <v>3.739133088485054</v>
       </c>
       <c r="J42" t="n">
-        <v>116.9300003051758</v>
+        <v>118.0699996948242</v>
       </c>
       <c r="K42" t="n">
-        <v>121.0999984741211</v>
+        <v>117.6699981689453</v>
       </c>
       <c r="L42" t="n">
-        <v>122.8899993896484</v>
+        <v>119.3000030517578</v>
       </c>
       <c r="M42" t="n">
-        <v>116.2099990844727</v>
+        <v>115</v>
       </c>
       <c r="N42" t="n">
         <v>4</v>
       </c>
       <c r="O42" t="n">
-        <v>122.1500015258789</v>
+        <v>116.9300003051758</v>
       </c>
       <c r="P42" t="n">
-        <v>-4.273435248052131</v>
+        <v>0.974941748630079</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
@@ -2955,37 +2955,37 @@
         <v>2</v>
       </c>
       <c r="F43" t="n">
-        <v>2.503601386119635</v>
+        <v>5.706024954921772</v>
       </c>
       <c r="G43" t="n">
-        <v>1.258361032098139</v>
+        <v>0.3286878885414234</v>
       </c>
       <c r="H43" t="n">
-        <v>-1.220782391436688</v>
+        <v>3.411459922790527</v>
       </c>
       <c r="I43" t="n">
-        <v>3.809904775269815</v>
+        <v>6.054613625147033</v>
       </c>
       <c r="J43" t="n">
-        <v>380.2999877929688</v>
+        <v>397.1000061035156</v>
       </c>
       <c r="K43" t="n">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L43" t="n">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="M43" t="n">
-        <v>376.6499938964844</v>
+        <v>379.0499877929688</v>
       </c>
       <c r="N43" t="n">
         <v>4</v>
       </c>
       <c r="O43" t="n">
-        <v>381.4500122070312</v>
+        <v>380.2999877929688</v>
       </c>
       <c r="P43" t="n">
-        <v>-0.3014875808781798</v>
+        <v>4.417570036760723</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
@@ -3014,37 +3014,37 @@
         <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>2.637511043034024</v>
+        <v>1.308047898643409</v>
       </c>
       <c r="G44" t="n">
-        <v>0.4446584246092474</v>
+        <v>0.258015075675938</v>
       </c>
       <c r="H44" t="n">
-        <v>1.313072135020896</v>
+        <v>0.1919660048452835</v>
       </c>
       <c r="I44" t="n">
-        <v>3.095935807029723</v>
+        <v>1.570114105416636</v>
       </c>
       <c r="J44" t="n">
-        <v>166.6600036621094</v>
+        <v>167.0200042724609</v>
       </c>
       <c r="K44" t="n">
-        <v>164.5</v>
+        <v>166.6999969482422</v>
       </c>
       <c r="L44" t="n">
-        <v>168.5</v>
+        <v>168.8399963378906</v>
       </c>
       <c r="M44" t="n">
-        <v>163.4400024414062</v>
+        <v>166.2299957275391</v>
       </c>
       <c r="N44" t="n">
         <v>4</v>
       </c>
       <c r="O44" t="n">
-        <v>164.1699981689453</v>
+        <v>166.6600036621094</v>
       </c>
       <c r="P44" t="n">
-        <v>1.516723835619239</v>
+        <v>0.2160090018247189</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
@@ -3073,37 +3073,37 @@
         <v>2</v>
       </c>
       <c r="F45" t="n">
-        <v>3.436283984257103</v>
+        <v>1.727759150321226</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.1904486976167532</v>
+        <v>0.6943303532578513</v>
       </c>
       <c r="H45" t="n">
-        <v>2.20314800181509</v>
+        <v>-0.6912052663108882</v>
       </c>
       <c r="I45" t="n">
-        <v>3.239665386105372</v>
+        <v>2.439024390243902</v>
       </c>
       <c r="J45" t="n">
-        <v>619.2999877929688</v>
+        <v>617.7999877929688</v>
       </c>
       <c r="K45" t="n">
-        <v>605.9500122070312</v>
+        <v>622.0999755859375</v>
       </c>
       <c r="L45" t="n">
-        <v>624.5999755859375</v>
+        <v>630</v>
       </c>
       <c r="M45" t="n">
-        <v>605</v>
+        <v>615</v>
       </c>
       <c r="N45" t="n">
         <v>4</v>
       </c>
       <c r="O45" t="n">
-        <v>603.8499755859375</v>
+        <v>619.2999877929688</v>
       </c>
       <c r="P45" t="n">
-        <v>2.558584554390276</v>
+        <v>-0.2422089503579077</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
@@ -3132,37 +3132,37 @@
         <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>0.9730679243587521</v>
+        <v>0.9463687058919491</v>
       </c>
       <c r="G46" t="n">
-        <v>1.96022618212905</v>
+        <v>0.9033622895866886</v>
       </c>
       <c r="H46" t="n">
-        <v>-1.649972017303653</v>
+        <v>-0.6837589448673433</v>
       </c>
       <c r="I46" t="n">
-        <v>2.991942955658996</v>
+        <v>1.866593093586124</v>
       </c>
       <c r="J46" t="n">
-        <v>348.7000122070312</v>
+        <v>348.6000061035156</v>
       </c>
       <c r="K46" t="n">
-        <v>354.5499877929688</v>
+        <v>351</v>
       </c>
       <c r="L46" t="n">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="M46" t="n">
-        <v>347.6000061035156</v>
+        <v>345.5499877929688</v>
       </c>
       <c r="N46" t="n">
         <v>4</v>
       </c>
       <c r="O46" t="n">
-        <v>354.5499877929688</v>
+        <v>348.7000122070312</v>
       </c>
       <c r="P46" t="n">
-        <v>-1.649972017303653</v>
+        <v>-0.02867969601797693</v>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
@@ -3191,37 +3191,37 @@
         <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>0.7445315389404988</v>
+        <v>-0.6550265966457947</v>
       </c>
       <c r="G47" t="n">
-        <v>2.229493563624844</v>
+        <v>3.394580747587613</v>
       </c>
       <c r="H47" t="n">
-        <v>0.7219939805660011</v>
+        <v>-0.3333346048990886</v>
       </c>
       <c r="I47" t="n">
-        <v>3.04184279182466</v>
+        <v>2.83581829274387</v>
       </c>
       <c r="J47" t="n">
-        <v>242.7400054931641</v>
+        <v>239.1999969482422</v>
       </c>
       <c r="K47" t="n">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L47" t="n">
-        <v>246.2700042724609</v>
+        <v>241.1499938964844</v>
       </c>
       <c r="M47" t="n">
-        <v>239</v>
+        <v>234.5</v>
       </c>
       <c r="N47" t="n">
         <v>4</v>
       </c>
       <c r="O47" t="n">
-        <v>244.4499969482422</v>
+        <v>242.7400054931641</v>
       </c>
       <c r="P47" t="n">
-        <v>-0.6995260693090475</v>
+        <v>-1.458353985668657</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
@@ -3250,37 +3250,37 @@
         <v>3</v>
       </c>
       <c r="F48" t="n">
-        <v>1.446965962363125</v>
+        <v>1.075376577712783</v>
       </c>
       <c r="G48" t="n">
-        <v>1.107674504034154</v>
+        <v>0.3015106047817211</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.7085112174027244</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>2.583254518068231</v>
+        <v>1.381051198314888</v>
       </c>
       <c r="J48" t="n">
-        <v>99.5</v>
+        <v>99.40000152587891</v>
       </c>
       <c r="K48" t="n">
-        <v>100.2099990844727</v>
+        <v>99.40000152587891</v>
       </c>
       <c r="L48" t="n">
-        <v>101.6600036621094</v>
+        <v>100.5699996948242</v>
       </c>
       <c r="M48" t="n">
-        <v>99.09999847412109</v>
+        <v>99.19999694824219</v>
       </c>
       <c r="N48" t="n">
         <v>4</v>
       </c>
       <c r="O48" t="n">
-        <v>100.2099990844727</v>
+        <v>99.5</v>
       </c>
       <c r="P48" t="n">
-        <v>-0.7085112174027244</v>
+        <v>-0.1005009790161746</v>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
@@ -3309,37 +3309,37 @@
         <v>1</v>
       </c>
       <c r="F49" t="n">
-        <v>1.165989023119272</v>
+        <v>3.609557702084393</v>
       </c>
       <c r="G49" t="n">
-        <v>1.527494908350306</v>
+        <v>-0.1575991655280884</v>
       </c>
       <c r="H49" t="n">
-        <v>0.5932277509004044</v>
+        <v>-0.970292296547701</v>
       </c>
       <c r="I49" t="n">
-        <v>2.735264964532704</v>
+        <v>3.446526839018309</v>
       </c>
       <c r="J49" t="n">
-        <v>983.5</v>
+        <v>990</v>
       </c>
       <c r="K49" t="n">
-        <v>977.7000122070312</v>
+        <v>999.7000122070312</v>
       </c>
       <c r="L49" t="n">
-        <v>993.4500122070312</v>
+        <v>1019</v>
       </c>
       <c r="M49" t="n">
-        <v>967</v>
+        <v>985.0499877929688</v>
       </c>
       <c r="N49" t="n">
         <v>4</v>
       </c>
       <c r="O49" t="n">
-        <v>982</v>
+        <v>983.5</v>
       </c>
       <c r="P49" t="n">
-        <v>0.1527494908350305</v>
+        <v>0.6609049313675649</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
@@ -3368,37 +3368,37 @@
         <v>3</v>
       </c>
       <c r="F50" t="n">
-        <v>3.900968975036962</v>
+        <v>2.411139029929017</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.325074388501383</v>
+        <v>0.8451408313612685</v>
       </c>
       <c r="H50" t="n">
-        <v>-1.276074742978336</v>
+        <v>-0.1225771903366491</v>
       </c>
       <c r="I50" t="n">
-        <v>3.564307934313802</v>
+        <v>3.284034578428609</v>
       </c>
       <c r="J50" t="n">
-        <v>40.22999954223633</v>
+        <v>40.7400016784668</v>
       </c>
       <c r="K50" t="n">
-        <v>40.75</v>
+        <v>40.79000091552734</v>
       </c>
       <c r="L50" t="n">
-        <v>41.54999923706055</v>
+        <v>41.20000076293945</v>
       </c>
       <c r="M50" t="n">
-        <v>40.11999893188477</v>
+        <v>39.88999938964844</v>
       </c>
       <c r="N50" t="n">
         <v>4</v>
       </c>
       <c r="O50" t="n">
-        <v>39.9900016784668</v>
+        <v>40.22999954223633</v>
       </c>
       <c r="P50" t="n">
-        <v>0.6001446704083577</v>
+        <v>1.267715988152155</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
@@ -3427,37 +3427,37 @@
         <v>1</v>
       </c>
       <c r="F51" t="n">
-        <v>1.870284605767774</v>
+        <v>0.2886893131327169</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.04437653903548901</v>
+        <v>1.845112587146703</v>
       </c>
       <c r="H51" t="n">
-        <v>0.8034461716008858</v>
+        <v>1.023017902813299</v>
       </c>
       <c r="I51" t="n">
-        <v>1.82509815133872</v>
+        <v>2.173913043478261</v>
       </c>
       <c r="J51" t="n">
-        <v>796.7000122070312</v>
+        <v>790</v>
       </c>
       <c r="K51" t="n">
-        <v>790.3499755859375</v>
+        <v>782</v>
       </c>
       <c r="L51" t="n">
-        <v>803.4000244140625</v>
+        <v>799</v>
       </c>
       <c r="M51" t="n">
-        <v>789</v>
+        <v>782</v>
       </c>
       <c r="N51" t="n">
         <v>4</v>
       </c>
       <c r="O51" t="n">
-        <v>788.6500244140625</v>
+        <v>796.7000122070312</v>
       </c>
       <c r="P51" t="n">
-        <v>1.020730050563251</v>
+        <v>-0.8409705164269757</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
@@ -3486,37 +3486,37 @@
         <v>3</v>
       </c>
       <c r="F52" t="n">
-        <v>3.372551413143382</v>
+        <v>7.662763943635848</v>
       </c>
       <c r="G52" t="n">
-        <v>5.788233139935662</v>
+        <v>-0.4819837596927151</v>
       </c>
       <c r="H52" t="n">
-        <v>-3.690003830304255</v>
+        <v>6.359644271432188</v>
       </c>
       <c r="I52" t="n">
-        <v>9.723609755335385</v>
+        <v>7.146336004986026</v>
       </c>
       <c r="J52" t="n">
-        <v>122.4100036621094</v>
+        <v>130.9499969482422</v>
       </c>
       <c r="K52" t="n">
-        <v>127.0999984741211</v>
+        <v>123.120002746582</v>
       </c>
       <c r="L52" t="n">
-        <v>131.8000030517578</v>
+        <v>131.7899932861328</v>
       </c>
       <c r="M52" t="n">
-        <v>120.120002746582</v>
+        <v>123</v>
       </c>
       <c r="N52" t="n">
         <v>4</v>
       </c>
       <c r="O52" t="n">
-        <v>127.5</v>
+        <v>122.4100036621094</v>
       </c>
       <c r="P52" t="n">
-        <v>-3.992153990502451</v>
+        <v>6.976548509634814</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
@@ -3545,37 +3545,37 @@
         <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>2.654245337359333</v>
+        <v>2.703751269175863</v>
       </c>
       <c r="G53" t="n">
-        <v>1.350409345290066</v>
+        <v>-1.039901441054104</v>
       </c>
       <c r="H53" t="n">
-        <v>1.263646737275741</v>
+        <v>-0.2111809922744657</v>
       </c>
       <c r="I53" t="n">
-        <v>4.059474201637957</v>
+        <v>1.646725505856155</v>
       </c>
       <c r="J53" t="n">
-        <v>649.0999755859375</v>
+        <v>661.5499877929688</v>
       </c>
       <c r="K53" t="n">
-        <v>641</v>
+        <v>662.9500122070312</v>
       </c>
       <c r="L53" t="n">
-        <v>661.3499755859375</v>
+        <v>666.6500244140625</v>
       </c>
       <c r="M53" t="n">
-        <v>635.5499877929688</v>
+        <v>655.8499755859375</v>
       </c>
       <c r="N53" t="n">
         <v>4</v>
       </c>
       <c r="O53" t="n">
-        <v>644.25</v>
+        <v>649.0999755859375</v>
       </c>
       <c r="P53" t="n">
-        <v>0.752809559322856</v>
+        <v>1.918042316330812</v>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
@@ -3604,37 +3604,37 @@
         <v>3</v>
       </c>
       <c r="F54" t="n">
-        <v>1.064537591483699</v>
+        <v>0.8299327097706172</v>
       </c>
       <c r="G54" t="n">
-        <v>0.8782402642631405</v>
+        <v>0.2409460976348458</v>
       </c>
       <c r="H54" t="n">
-        <v>-0.724254113891196</v>
+        <v>-0.2935306480361908</v>
       </c>
       <c r="I54" t="n">
-        <v>1.959991288417775</v>
+        <v>1.073465280107347</v>
       </c>
       <c r="J54" t="n">
-        <v>1494.099975585938</v>
+        <v>1494.599975585938</v>
       </c>
       <c r="K54" t="n">
-        <v>1505</v>
+        <v>1499</v>
       </c>
       <c r="L54" t="n">
-        <v>1519</v>
+        <v>1506.5</v>
       </c>
       <c r="M54" t="n">
-        <v>1489.800048828125</v>
+        <v>1490.5</v>
       </c>
       <c r="N54" t="n">
         <v>4</v>
       </c>
       <c r="O54" t="n">
-        <v>1503</v>
+        <v>1494.099975585938</v>
       </c>
       <c r="P54" t="n">
-        <v>-0.5921506596182634</v>
+        <v>0.03346496273142072</v>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
@@ -3663,37 +3663,37 @@
         <v>4</v>
       </c>
       <c r="F55" t="n">
-        <v>2.591952565243093</v>
+        <v>3.646651308691142</v>
       </c>
       <c r="G55" t="n">
-        <v>2.241426056044917</v>
+        <v>0.3266371806232418</v>
       </c>
       <c r="H55" t="n">
-        <v>3.075374430747488</v>
+        <v>1.866537985197942</v>
       </c>
       <c r="I55" t="n">
-        <v>4.944199190199913</v>
+        <v>3.986309257483953</v>
       </c>
       <c r="J55" t="n">
-        <v>205.1199951171875</v>
+        <v>210.6600036621094</v>
       </c>
       <c r="K55" t="n">
-        <v>199</v>
+        <v>206.8000030517578</v>
       </c>
       <c r="L55" t="n">
-        <v>207.8000030517578</v>
+        <v>212.6000061035156</v>
       </c>
       <c r="M55" t="n">
-        <v>198.0099945068359</v>
+        <v>204.4499969482422</v>
       </c>
       <c r="N55" t="n">
         <v>4</v>
       </c>
       <c r="O55" t="n">
-        <v>202.5500030517578</v>
+        <v>205.1199951171875</v>
       </c>
       <c r="P55" t="n">
-        <v>1.268818576503786</v>
+        <v>2.700862264430536</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
@@ -3722,37 +3722,37 @@
         <v>2</v>
       </c>
       <c r="F56" t="n">
-        <v>3.864736851610484</v>
+        <v>0.8617952710538446</v>
       </c>
       <c r="G56" t="n">
-        <v>0.9339742843941038</v>
+        <v>0.9575462425505799</v>
       </c>
       <c r="H56" t="n">
-        <v>1.064515882922757</v>
+        <v>-0.3488760163527466</v>
       </c>
       <c r="I56" t="n">
-        <v>4.843952405823266</v>
+        <v>1.836930977154414</v>
       </c>
       <c r="J56" t="n">
-        <v>31.32999992370605</v>
+        <v>31.42000007629395</v>
       </c>
       <c r="K56" t="n">
-        <v>31</v>
+        <v>31.53000068664551</v>
       </c>
       <c r="L56" t="n">
-        <v>32.25</v>
+        <v>31.60000038146973</v>
       </c>
       <c r="M56" t="n">
-        <v>30.76000022888184</v>
+        <v>31.03000068664551</v>
       </c>
       <c r="N56" t="n">
         <v>4</v>
       </c>
       <c r="O56" t="n">
-        <v>31.04999923706055</v>
+        <v>31.32999992370605</v>
       </c>
       <c r="P56" t="n">
-        <v>0.9017735701304159</v>
+        <v>0.2872650903512815</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
@@ -3781,37 +3781,37 @@
         <v>11</v>
       </c>
       <c r="F57" t="n">
-        <v>2.020209804504464</v>
+        <v>1.323830127097015</v>
       </c>
       <c r="G57" t="n">
-        <v>2.222215372036072</v>
+        <v>0.9164985273403479</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.7077921746059006</v>
+        <v>-1.608038698283415</v>
       </c>
       <c r="I57" t="n">
-        <v>4.338843626578981</v>
+        <v>2.261051154975122</v>
       </c>
       <c r="J57" t="n">
-        <v>9.819999694824219</v>
+        <v>9.789999961853027</v>
       </c>
       <c r="K57" t="n">
-        <v>9.890000343322754</v>
+        <v>9.949999809265137</v>
       </c>
       <c r="L57" t="n">
-        <v>10.10000038146973</v>
+        <v>9.949999809265137</v>
       </c>
       <c r="M57" t="n">
-        <v>9.680000305175781</v>
+        <v>9.729999542236328</v>
       </c>
       <c r="N57" t="n">
         <v>4</v>
       </c>
       <c r="O57" t="n">
-        <v>9.899999618530273</v>
+        <v>9.819999694824219</v>
       </c>
       <c r="P57" t="n">
-        <v>-0.8080800685720759</v>
+        <v>-0.3054962719296542</v>
       </c>
       <c r="Q57" t="inlineStr">
         <is>
@@ -3840,37 +3840,37 @@
         <v>6</v>
       </c>
       <c r="F58" t="n">
-        <v>0.5641496920634254</v>
+        <v>1.500411911818039</v>
       </c>
       <c r="G58" t="n">
-        <v>2.949712772484301</v>
+        <v>1.368510816443314</v>
       </c>
       <c r="H58" t="n">
-        <v>-0.7364925687073196</v>
+        <v>1.070836413528513</v>
       </c>
       <c r="I58" t="n">
-        <v>3.620661581670699</v>
+        <v>2.908728999236933</v>
       </c>
       <c r="J58" t="n">
-        <v>60.65000152587891</v>
+        <v>61.34999847412109</v>
       </c>
       <c r="K58" t="n">
-        <v>61.09999847412109</v>
+        <v>60.70000076293945</v>
       </c>
       <c r="L58" t="n">
-        <v>62.38999938964844</v>
+        <v>61.56000137329102</v>
       </c>
       <c r="M58" t="n">
-        <v>60.20999908447266</v>
+        <v>59.81999969482422</v>
       </c>
       <c r="N58" t="n">
         <v>4</v>
       </c>
       <c r="O58" t="n">
-        <v>62.04000091552734</v>
+        <v>60.65000152587891</v>
       </c>
       <c r="P58" t="n">
-        <v>-2.240488989581154</v>
+        <v>1.154158170867488</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
@@ -3899,37 +3899,37 @@
         <v>5</v>
       </c>
       <c r="F59" t="n">
-        <v>2.970962646297403</v>
+        <v>4.790421023423904</v>
       </c>
       <c r="G59" t="n">
-        <v>2.717759224738144</v>
+        <v>3.127074662040468</v>
       </c>
       <c r="H59" t="n">
-        <v>3.699871520861114</v>
+        <v>1.762440825910898</v>
       </c>
       <c r="I59" t="n">
-        <v>5.847646832249104</v>
+        <v>8.173073805547515</v>
       </c>
       <c r="J59" t="n">
-        <v>120.2399978637695</v>
+        <v>124.1399993896484</v>
       </c>
       <c r="K59" t="n">
-        <v>115.9499969482422</v>
+        <v>121.9899978637695</v>
       </c>
       <c r="L59" t="n">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M59" t="n">
-        <v>115.2600021362305</v>
+        <v>116.4800033569336</v>
       </c>
       <c r="N59" t="n">
         <v>4</v>
       </c>
       <c r="O59" t="n">
-        <v>118.4800033569336</v>
+        <v>120.2399978637695</v>
       </c>
       <c r="P59" t="n">
-        <v>1.485478103451573</v>
+        <v>3.243514300705129</v>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
@@ -3958,37 +3958,37 @@
         <v>1</v>
       </c>
       <c r="F60" t="n">
-        <v>0.3155104353281624</v>
+        <v>3.938187551971924</v>
       </c>
       <c r="G60" t="n">
-        <v>2.920473772263068</v>
+        <v>-0.9388541922015162</v>
       </c>
       <c r="H60" t="n">
-        <v>-2.336907518467294</v>
+        <v>1.747337885818294</v>
       </c>
       <c r="I60" t="n">
-        <v>3.333333333333333</v>
+        <v>2.971435909168597</v>
       </c>
       <c r="J60" t="n">
-        <v>1203.599975585938</v>
+        <v>1240.300048828125</v>
       </c>
       <c r="K60" t="n">
-        <v>1232.400024414062</v>
+        <v>1219</v>
       </c>
       <c r="L60" t="n">
-        <v>1240</v>
+        <v>1251</v>
       </c>
       <c r="M60" t="n">
-        <v>1200</v>
+        <v>1214.900024414062</v>
       </c>
       <c r="N60" t="n">
         <v>4</v>
       </c>
       <c r="O60" t="n">
-        <v>1236.099975585938</v>
+        <v>1203.599975585938</v>
       </c>
       <c r="P60" t="n">
-        <v>-2.629237168667875</v>
+        <v>3.04919192311558</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
@@ -4017,37 +4017,37 @@
         <v>3</v>
       </c>
       <c r="F61" t="n">
-        <v>2.544554810008303</v>
+        <v>1.842468942869762</v>
       </c>
       <c r="G61" t="n">
-        <v>1.696360374442688</v>
+        <v>0.5834466243190944</v>
       </c>
       <c r="H61" t="n">
-        <v>0.9767422934835271</v>
+        <v>0.7621951219512195</v>
       </c>
       <c r="I61" t="n">
-        <v>4.314097830563359</v>
+        <v>2.440152554898649</v>
       </c>
       <c r="J61" t="n">
-        <v>1302.599975585938</v>
+        <v>1322</v>
       </c>
       <c r="K61" t="n">
-        <v>1290</v>
+        <v>1312</v>
       </c>
       <c r="L61" t="n">
-        <v>1317.800048828125</v>
+        <v>1326.599975585938</v>
       </c>
       <c r="M61" t="n">
-        <v>1263.300048828125</v>
+        <v>1295</v>
       </c>
       <c r="N61" t="n">
         <v>4</v>
       </c>
       <c r="O61" t="n">
-        <v>1285.099975585938</v>
+        <v>1302.599975585938</v>
       </c>
       <c r="P61" t="n">
-        <v>1.361761756475089</v>
+        <v>1.489330936409388</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
@@ -4076,37 +4076,37 @@
         <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>1.780539565945264</v>
+        <v>2.147468801179892</v>
       </c>
       <c r="G62" t="n">
-        <v>0.3105590062111801</v>
+        <v>-0.4220474608460016</v>
       </c>
       <c r="H62" t="n">
-        <v>-0.148736002453107</v>
+        <v>-0.1762265064677254</v>
       </c>
       <c r="I62" t="n">
-        <v>2.097612897926402</v>
+        <v>1.718169848116891</v>
       </c>
       <c r="J62" t="n">
-        <v>241.6799926757812</v>
+        <v>243.5700073242188</v>
       </c>
       <c r="K62" t="n">
-        <v>242.0399932861328</v>
+        <v>244</v>
       </c>
       <c r="L62" t="n">
-        <v>245.8000030517578</v>
+        <v>246.8699951171875</v>
       </c>
       <c r="M62" t="n">
-        <v>240.75</v>
+        <v>242.6999969482422</v>
       </c>
       <c r="N62" t="n">
         <v>4</v>
       </c>
       <c r="O62" t="n">
-        <v>241.5</v>
+        <v>241.6799926757812</v>
       </c>
       <c r="P62" t="n">
-        <v>0.07453112868788819</v>
+        <v>0.7820319040529738</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
@@ -4135,28 +4135,28 @@
         <v>171</v>
       </c>
       <c r="F63" t="n">
-        <v>1.523704673962311</v>
+        <v>0.6772056652562117</v>
       </c>
       <c r="G63" t="n">
-        <v>0.5079015579874371</v>
+        <v>1.185096459424762</v>
       </c>
       <c r="H63" t="n">
-        <v>0</v>
+        <v>0.1694846214904517</v>
       </c>
       <c r="I63" t="n">
-        <v>2.041977467320019</v>
+        <v>1.884636889734227</v>
       </c>
       <c r="J63" t="n">
-        <v>17.71999931335449</v>
+        <v>17.72999954223633</v>
       </c>
       <c r="K63" t="n">
-        <v>17.71999931335449</v>
+        <v>17.70000076293945</v>
       </c>
       <c r="L63" t="n">
-        <v>17.98999977111816</v>
+        <v>17.84000015258789</v>
       </c>
       <c r="M63" t="n">
-        <v>17.6299991607666</v>
+        <v>17.51000022888184</v>
       </c>
       <c r="N63" t="n">
         <v>4</v>
@@ -4165,11 +4165,129 @@
         <v>17.71999931335449</v>
       </c>
       <c r="P63" t="n">
-        <v>0</v>
+        <v>0.05643470242292487</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
           <t>n.v.saikumar9@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>HARSH VARDHAN</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>STERTOOLS</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>356.45</v>
+      </c>
+      <c r="E64" t="n">
+        <v>5</v>
+      </c>
+      <c r="F64" t="n">
+        <v>3.077920034946162</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.9881703720336572</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.4996736724608087</v>
+      </c>
+      <c r="I64" t="n">
+        <v>4.106671316203346</v>
+      </c>
+      <c r="J64" t="n">
+        <v>311.75</v>
+      </c>
+      <c r="K64" t="n">
+        <v>310.2000122070312</v>
+      </c>
+      <c r="L64" t="n">
+        <v>318.1499938964844</v>
+      </c>
+      <c r="M64" t="n">
+        <v>305.6000061035156</v>
+      </c>
+      <c r="N64" t="n">
+        <v>3</v>
+      </c>
+      <c r="O64" t="n">
+        <v>308.6499938964844</v>
+      </c>
+      <c r="P64" t="n">
+        <v>1.004375883628013</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>nunna.harshavardhan2001@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>HARSH VARDHAN</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>TATAMOTORS</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>873.5667</v>
+      </c>
+      <c r="E65" t="n">
+        <v>3</v>
+      </c>
+      <c r="F65" t="n">
+        <v>2.703751269175863</v>
+      </c>
+      <c r="G65" t="n">
+        <v>-1.039901441054104</v>
+      </c>
+      <c r="H65" t="n">
+        <v>-0.2111809922744657</v>
+      </c>
+      <c r="I65" t="n">
+        <v>1.646725505856155</v>
+      </c>
+      <c r="J65" t="n">
+        <v>661.5499877929688</v>
+      </c>
+      <c r="K65" t="n">
+        <v>662.9500122070312</v>
+      </c>
+      <c r="L65" t="n">
+        <v>666.6500244140625</v>
+      </c>
+      <c r="M65" t="n">
+        <v>655.8499755859375</v>
+      </c>
+      <c r="N65" t="n">
+        <v>3</v>
+      </c>
+      <c r="O65" t="n">
+        <v>649.0999755859375</v>
+      </c>
+      <c r="P65" t="n">
+        <v>1.918042316330812</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>nunna.harshavardhan2001@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>